<commit_message>
create desktop project for shops
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sotiris\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sotiris\Documents\GitHub\Foodisimo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="Εργασίες" sheetId="6" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="Προβολή εβδομάδας" sheetId="5" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Εργασίες!$F$3:$F$18</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Εργασίες!$3:$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Εργασίες!$F$2:$F$18</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Εργασίες!$2:$2</definedName>
     <definedName name="ΑρΕβδΜήνα">MONTH(DATEVALUE(" 1/ "&amp;'Προβολή εβδομάδας'!ΕβδΜήνα))</definedName>
     <definedName name="ΑρΜΜήνα">MONTH(DATEVALUE(" 1/ "&amp;ΜΜήνας))</definedName>
     <definedName name="Εβδ2Μήνα">'Προβολή μήνα'!$B$8:$H$9</definedName>
@@ -36,12 +36,11 @@
     <definedName name="ΤίτλοςΣτήλης1">Εργασίες[[#Headers],[ΠΕΡΙΓΡΑΦΗ]]</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>ΠΡΟΒΟΛΗ ΜΗΝΑ</t>
   </si>
@@ -109,9 +108,6 @@
     <t>Feature Εισαγωγή Νέου Καταστήματος Admin</t>
   </si>
   <si>
-    <t xml:space="preserve"> ΕΡΓΑΣΙΕΣ ΓIA V.0.1</t>
-  </si>
-  <si>
     <t>ΑΝΑΘΕΣΗ ΣΕ</t>
   </si>
   <si>
@@ -176,6 +172,9 @@
   </si>
   <si>
     <t>Front-End, Back-End</t>
+  </si>
+  <si>
+    <t>Version</t>
   </si>
 </sst>
 </file>
@@ -184,7 +183,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -396,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -503,15 +502,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thick">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thick">
         <color theme="0"/>
@@ -546,6 +536,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -596,11 +619,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
@@ -654,7 +676,7 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,34 +691,58 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="6" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="11" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="2" borderId="11" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="11" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="8" borderId="11" xfId="20" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="9" borderId="11" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="10" borderId="10" xfId="22" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="12" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="12" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="12" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="12" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="12" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="12" xfId="20" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="9" borderId="12" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="10" borderId="11" xfId="22" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,7 +771,61 @@
     <cellStyle name="Σκιασμένη σημείωση ημέρας προβολής εβδομάδας" xfId="18"/>
     <cellStyle name="Χρώμα εργασίας" xfId="6"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -949,9 +1049,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Πρόγραμμα σπουδαστή" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="9"/>
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -971,7 +1071,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>236220</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="254557"/>
@@ -983,6 +1083,104 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13472160" y="990600"/>
+          <a:ext cx="184731" cy="254557"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="el-GR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="254557"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14813280" y="548640"/>
+          <a:ext cx="184731" cy="254557"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="el-GR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="254557"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14813280" y="1623060"/>
           <a:ext cx="184731" cy="254557"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1150,13 +1348,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Εργασίες" displayName="Εργασίες" ref="B3:E21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="B3:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Εργασίες" displayName="Εργασίες" ref="B2:E21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="B2:E21"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ΠΕΡΙΓΡΑΦΗ" dataDxfId="3" dataCellStyle="Περιγραφή της εργασίας"/>
-    <tableColumn id="3" name="ΑΝΑΘΕΣΗ ΣΕ" dataDxfId="2" dataCellStyle="Περιγραφή της εργασίας"/>
-    <tableColumn id="4" name="ΑΠΌ" dataDxfId="1" dataCellStyle="Περιγραφή της εργασίας"/>
-    <tableColumn id="2" name="ΕΩΣ" dataDxfId="0" dataCellStyle="Ημερομηνία"/>
+    <tableColumn id="1" name="ΠΕΡΙΓΡΑΦΗ" dataDxfId="11" dataCellStyle="Περιγραφή της εργασίας"/>
+    <tableColumn id="3" name="ΑΝΑΘΕΣΗ ΣΕ" dataDxfId="10" dataCellStyle="Περιγραφή της εργασίας"/>
+    <tableColumn id="4" name="ΑΠΌ" dataDxfId="9" dataCellStyle="Περιγραφή της εργασίας"/>
+    <tableColumn id="2" name="ΕΩΣ" dataDxfId="8" dataCellStyle="Ημερομηνία"/>
+  </tableColumns>
+  <tableStyleInfo name="Πρόγραμμα σπουδαστή" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:A21" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5" headerRowCellStyle="Χρώμα εργασίας">
+  <autoFilter ref="A2:A21"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Version"/>
+  </tableColumns>
+  <tableStyleInfo name="Πρόγραμμα σπουδαστή" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="F2:F21" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1" headerRowCellStyle="Χρώμα εργασίας">
+  <autoFilter ref="F2:F21"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="ΏΡΕΣ"/>
   </tableColumns>
   <tableStyleInfo name="Πρόγραμμα σπουδαστή" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1453,402 +1671,453 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.59765625" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" style="39" customWidth="1"/>
     <col min="2" max="2" width="55.8984375" customWidth="1"/>
     <col min="3" max="3" width="25.69921875" customWidth="1"/>
-    <col min="4" max="4" width="27.69921875" customWidth="1"/>
-    <col min="5" max="5" width="27.09765625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="27.69921875" customWidth="1"/>
+    <col min="4" max="4" width="22.3984375" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.09765625" customWidth="1"/>
+    <col min="7" max="7" width="23.19921875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" ht="35.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-    </row>
-    <row r="3" spans="1:7" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="D2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="22">
+        <v>43777</v>
+      </c>
+      <c r="E3" s="19">
+        <v>43786</v>
+      </c>
+      <c r="F3" s="25">
+        <v>5</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="21">
+        <v>43781</v>
+      </c>
+      <c r="E4" s="15">
+        <v>43783</v>
+      </c>
+      <c r="F4" s="26">
+        <v>9</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="21">
+        <v>43784</v>
+      </c>
+      <c r="E5" s="15">
+        <v>43786</v>
+      </c>
+      <c r="F5" s="27">
+        <v>10</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="21">
+        <v>43788</v>
+      </c>
+      <c r="E6" s="15">
+        <v>43788</v>
+      </c>
+      <c r="F6" s="26">
+        <v>2</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="21">
+        <v>43782</v>
+      </c>
+      <c r="E8" s="15">
+        <v>43793</v>
+      </c>
+      <c r="F8" s="36">
+        <v>50</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="21">
+        <v>43794</v>
+      </c>
+      <c r="E9" s="15">
+        <v>43798</v>
+      </c>
+      <c r="F9" s="37">
+        <v>18</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="21">
+        <v>43799</v>
+      </c>
+      <c r="E10" s="15">
+        <v>43802</v>
+      </c>
+      <c r="F10" s="36">
+        <v>18</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="22">
+        <v>43783</v>
+      </c>
+      <c r="E11" s="19">
+        <v>43817</v>
+      </c>
+      <c r="F11" s="37">
+        <v>45</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="22">
+        <v>43818</v>
+      </c>
+      <c r="E12" s="19">
+        <v>43827</v>
+      </c>
+      <c r="F12" s="36">
+        <v>4</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="21">
+        <v>43828</v>
+      </c>
+      <c r="E13" s="15">
+        <v>43863</v>
+      </c>
+      <c r="F13" s="37">
+        <v>4</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="21">
+        <v>43788</v>
+      </c>
+      <c r="E14" s="15">
+        <v>43789</v>
+      </c>
+      <c r="F14" s="36">
+        <v>2</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="21">
+        <v>43790</v>
+      </c>
+      <c r="E15" s="15">
+        <v>43791</v>
+      </c>
+      <c r="F15" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="25" t="s">
+      <c r="G15" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="23">
-        <v>43777</v>
-      </c>
-      <c r="E4" s="20">
-        <v>43786</v>
-      </c>
-      <c r="F4" s="29">
-        <v>5</v>
-      </c>
-      <c r="G4" s="33" t="s">
+      <c r="D16" s="21">
+        <v>43792</v>
+      </c>
+      <c r="E16" s="15">
+        <v>43796</v>
+      </c>
+      <c r="F16" s="36">
+        <v>3</v>
+      </c>
+      <c r="G16" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="22">
-        <v>43781</v>
-      </c>
-      <c r="E5" s="16">
-        <v>43783</v>
-      </c>
-      <c r="F5" s="30">
-        <v>9</v>
-      </c>
-      <c r="G5" s="33" t="s">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="21">
+        <v>43797</v>
+      </c>
+      <c r="E17" s="15">
+        <v>43798</v>
+      </c>
+      <c r="F17" s="37">
+        <v>2</v>
+      </c>
+      <c r="G17" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="22">
-        <v>43784</v>
-      </c>
-      <c r="E6" s="16">
-        <v>43786</v>
-      </c>
-      <c r="F6" s="31">
-        <v>10</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="22">
-        <v>43788</v>
-      </c>
-      <c r="E7" s="16">
-        <v>43788</v>
-      </c>
-      <c r="F7" s="30">
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="21">
+        <v>43799</v>
+      </c>
+      <c r="E18" s="15">
+        <v>43799</v>
+      </c>
+      <c r="F18" s="36">
         <v>2</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="22">
-        <v>43782</v>
-      </c>
-      <c r="E8" s="16">
-        <v>43793</v>
-      </c>
-      <c r="F8" s="31">
-        <v>50</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="22">
-        <v>43794</v>
-      </c>
-      <c r="E9" s="16">
-        <v>43798</v>
-      </c>
-      <c r="F9" s="30">
-        <v>18</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="22">
-        <v>43799</v>
-      </c>
-      <c r="E10" s="16">
-        <v>43802</v>
-      </c>
-      <c r="F10" s="31">
-        <v>18</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="23">
-        <v>43783</v>
-      </c>
-      <c r="E11" s="20">
-        <v>43817</v>
-      </c>
-      <c r="F11" s="32">
-        <v>45</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="23">
-        <v>43818</v>
-      </c>
-      <c r="E12" s="20">
-        <v>43827</v>
-      </c>
-      <c r="F12" s="29">
-        <v>4</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="22">
-        <v>43828</v>
-      </c>
-      <c r="E13" s="16">
-        <v>43863</v>
-      </c>
-      <c r="F13" s="30">
-        <v>4</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="22">
-        <v>43788</v>
-      </c>
-      <c r="E14" s="16">
-        <v>43789</v>
-      </c>
-      <c r="F14" s="31">
-        <v>2</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="22">
-        <v>43790</v>
-      </c>
-      <c r="E15" s="16">
-        <v>43791</v>
-      </c>
-      <c r="F15" s="30">
-        <v>1</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="22">
-        <v>43792</v>
-      </c>
-      <c r="E16" s="16">
-        <v>43796</v>
-      </c>
-      <c r="F16" s="31">
-        <v>3</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="22">
-        <v>43797</v>
-      </c>
-      <c r="E17" s="16">
-        <v>43798</v>
-      </c>
-      <c r="F17" s="30">
-        <v>2</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="22">
-        <v>43799</v>
-      </c>
-      <c r="E18" s="16">
-        <v>43799</v>
-      </c>
-      <c r="F18" s="31">
-        <v>2</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
+      <c r="G18" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="F3:F18"/>
-  <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
-  </mergeCells>
-  <dataValidations count="5">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Εισαγάγετε εργασίες σε αυτό το φύλλο εργασίας. Μπορείτε να βρείτε μια προβολή μήνα και εβδομάδας αυτών των εργασιών στα αντίστοιχα φύλλα εργασίας &quot;Προβολή μήνα&quot; και &quot;Προβολή εβδομάδας&quot; αυτού του βιβλίου εργασίας" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Μεταβείτε στο φύλλο εργασίας &quot;Προβολή μήνα&quot; των εργασιών σε αυτό το φύλλο εργασίας επιλέγοντας την υπερ-σύνδεση σε αυτό το κελί" sqref="B1:D1 F1:G1"/>
+  <dataValidations xWindow="121" yWindow="500" count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Μεταβείτε στο φύλλο εργασίας &quot;Προβολή μήνα&quot; των εργασιών σε αυτό το φύλλο εργασίας επιλέγοντας την υπερ-σύνδεση σε αυτό το κελί" sqref="A1:D1 F1:G1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Μεταβείτε στο φύλλο εργασίας &quot;Προβολή εβδομάδας&quot; των εργασιών σε αυτό το φύλλο εργασίας επιλέγοντας την υπερ-σύνδεση σε αυτό το κελί" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Εισαγάγετε την περιγραφή για την εργασία ανάθεση σε αυτή τη στήλη" sqref="B3:D4 F3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Εισαγάγετε την προθεσμία παράδοσης σε αυτή τη στήλη" sqref="E3:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Εισαγάγετε την περιγραφή για την εργασία ανάθεση σε αυτή τη στήλη" sqref="A2:D3 F2:G3 A4:A13"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Εισαγάγετε την προθεσμία παράδοσης σε αυτή τη στήλη" sqref="E2:E3"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B1" location="'Προβολή μήνα'!A1" tooltip="Κάντε κλικ για να δείτε το μηνιαίο πρόγραμμα" display="ΠΡΟΒΟΛΗ ΜΗΝΑ"/>
     <hyperlink ref="E1" location="'Προβολή εβδομάδας'!A1" tooltip="Κάντε κλικ για να δείτε το εβδομαδιαίο πρόγραμμα" display="ΠΡΟΒΟΛΗ ΕΒΔΟΜΑΔΑΣ"/>
+    <hyperlink ref="A1" location="'Προβολή μήνα'!A1" tooltip="Κάντε κλικ για να δείτε το μηνιαίο πρόγραμμα" display="ΠΡΟΒΟΛΗ ΜΗΝΑ"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1857,8 +2126,10 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1885,10 +2156,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1901,405 +2172,405 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>9</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <f ca="1">YEAR(TODAY())</f>
         <v>2019</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:11" ht="24.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="str">
+      <c r="B6" s="3" t="str">
         <f t="shared" ref="B6:H6" ca="1" si="0">IF(WEEKDAY(DATEVALUE(" 1/ "&amp;ΜΜήνας&amp;" / "&amp;ΜηνΈτους)-1)=COLUMN(A$2),1,IF(LEN(A6)&gt;0,A6+1,""))</f>
         <v/>
       </c>
-      <c r="C6" s="4" t="str">
+      <c r="C6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="D6" s="4" t="str">
+      <c r="D6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="E6" s="4" t="str">
+      <c r="E6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="F6" s="4" t="str">
+      <c r="F6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="G6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="4" t="str">
         <f ca="1">IF(LEN(B6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,B6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C7" s="5" t="str">
+      <c r="C7" s="4" t="str">
         <f ca="1">IF(LEN(C6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,C6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D7" s="5" t="str">
+      <c r="D7" s="4" t="str">
         <f ca="1">IF(LEN(D6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,D6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E7" s="5" t="str">
+      <c r="E7" s="4" t="str">
         <f ca="1">IF(LEN(E6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,E6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F7" s="5" t="str">
+      <c r="F7" s="4" t="str">
         <f ca="1">IF(LEN(F6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,F6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G7" s="5" t="str">
+      <c r="G7" s="4" t="str">
         <f ca="1">IF(LEN(G6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,G6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H7" s="5" t="str">
+      <c r="H7" s="4" t="str">
         <f ca="1">IF(LEN(H6)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,H6))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="K7" s="18"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <f ca="1">IF(LEN(H6)&gt;0,IF(H6=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",H6+1),"")</f>
         <v>2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" ref="C8:H8" ca="1" si="1">IF(LEN(B8)&gt;0,IF(B8=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",B8+1),"")</f>
         <v>3</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="str">
+      <c r="B9" s="5" t="str">
         <f ca="1">IF(LEN(B8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,B8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C9" s="6" t="str">
+      <c r="C9" s="5" t="str">
         <f ca="1">IF(LEN(C8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,C8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D9" s="6" t="str">
+      <c r="D9" s="5" t="str">
         <f ca="1">IF(LEN(D8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,D8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E9" s="6" t="str">
+      <c r="E9" s="5" t="str">
         <f ca="1">IF(LEN(E8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,E8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F9" s="6" t="str">
+      <c r="F9" s="5" t="str">
         <f ca="1">IF(LEN(F8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,F8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G9" s="6" t="str">
+      <c r="G9" s="5" t="str">
         <f ca="1">IF(LEN(G8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,G8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H9" s="6" t="str">
+      <c r="H9" s="5" t="str">
         <f ca="1">IF(LEN(H8)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,H8))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <f ca="1">IF(LEN(H8)&gt;0,IF(H8=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",H8+1),"")</f>
         <v>9</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f t="shared" ref="C10:H10" ca="1" si="2">IF(LEN(B10)&gt;0,IF(B10=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",B10+1),"")</f>
         <v>10</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
         <v>11</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <f t="shared" ca="1" si="2"/>
         <v>12</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f t="shared" ca="1" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="4" t="str">
         <f ca="1">IF(LEN(B10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,B10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C11" s="5" t="str">
+      <c r="C11" s="4" t="str">
         <f ca="1">IF(LEN(C10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,C10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D11" s="5" t="str">
+      <c r="D11" s="4" t="str">
         <f ca="1">IF(LEN(D10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,D10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E11" s="4" t="str">
         <f ca="1">IF(LEN(E10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,E10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F11" s="5" t="str">
+      <c r="F11" s="4" t="str">
         <f ca="1">IF(LEN(F10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,F10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G11" s="5" t="str">
+      <c r="G11" s="4" t="str">
         <f ca="1">IF(LEN(G10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,G10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H11" s="5" t="str">
+      <c r="H11" s="4" t="str">
         <f ca="1">IF(LEN(H10)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,H10))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f ca="1">IF(LEN(H10)&gt;0,IF(H10=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",H10+1),"")</f>
         <v>16</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f t="shared" ref="C12:H12" ca="1" si="3">IF(LEN(B12)&gt;0,IF(B12=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",B12+1),"")</f>
         <v>17</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <f t="shared" ca="1" si="3"/>
         <v>18</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f t="shared" ca="1" si="3"/>
         <v>19</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <f t="shared" ca="1" si="3"/>
         <v>21</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <f t="shared" ca="1" si="3"/>
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="str">
+      <c r="B13" s="5" t="str">
         <f ca="1">IF(LEN(B12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,B12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C13" s="6" t="str">
+      <c r="C13" s="5" t="str">
         <f ca="1">IF(LEN(C12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,C12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D13" s="6" t="str">
+      <c r="D13" s="5" t="str">
         <f ca="1">IF(LEN(D12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,D12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E13" s="6" t="str">
+      <c r="E13" s="5" t="str">
         <f ca="1">IF(LEN(E12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,E12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F13" s="6" t="str">
+      <c r="F13" s="5" t="str">
         <f ca="1">IF(LEN(F12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,F12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G13" s="6" t="str">
+      <c r="G13" s="5" t="str">
         <f ca="1">IF(LEN(G12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,G12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H13" s="6" t="str">
+      <c r="H13" s="5" t="str">
         <f ca="1">IF(LEN(H12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,H12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <f ca="1">IF(LEN(H12)&gt;0,IF(H12=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",H12+1),"")</f>
         <v>23</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <f t="shared" ref="C14:H14" ca="1" si="4">IF(LEN(B14)&gt;0,IF(B14=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",B14+1),"")</f>
         <v>24</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <f t="shared" ca="1" si="4"/>
         <v>25</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" ca="1" si="4"/>
         <v>26</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <f t="shared" ca="1" si="4"/>
         <v>27</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" ca="1" si="4"/>
         <v>28</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f t="shared" ca="1" si="4"/>
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="str">
+      <c r="B15" s="4" t="str">
         <f ca="1">IF(LEN(B14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,B14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C15" s="5" t="str">
+      <c r="C15" s="4" t="str">
         <f ca="1">IF(LEN(C14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,C14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D15" s="5" t="str">
+      <c r="D15" s="4" t="str">
         <f ca="1">IF(LEN(D14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,D14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E15" s="5" t="str">
+      <c r="E15" s="4" t="str">
         <f ca="1">IF(LEN(E14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,E14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F15" s="5" t="str">
+      <c r="F15" s="4" t="str">
         <f ca="1">IF(LEN(F14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,F14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G15" s="5" t="str">
+      <c r="G15" s="4" t="str">
         <f ca="1">IF(LEN(G14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,G14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H15" s="5" t="str">
+      <c r="H15" s="4" t="str">
         <f ca="1">IF(LEN(H14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,H14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <f ca="1">IF(LEN(H14)&gt;0,IF(H14=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",H14+1),"")</f>
         <v>30</v>
       </c>
-      <c r="C16" s="7" t="str">
+      <c r="C16" s="6" t="str">
         <f t="shared" ref="C16:H16" ca="1" si="5">IF(LEN(B16)&gt;0,IF(B16=DAY(DATE(ΜηνΈτους,ΑρΜΜήνα+1,0)),"",B16+1),"")</f>
         <v/>
       </c>
-      <c r="D16" s="7" t="str">
+      <c r="D16" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="E16" s="7" t="str">
+      <c r="E16" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="F16" s="7" t="str">
+      <c r="F16" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="G16" s="7" t="str">
+      <c r="G16" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="H16" s="7" t="str">
+      <c r="H16" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="str">
+      <c r="B17" s="5" t="str">
         <f ca="1">IF(LEN(B16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,B16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C17" s="6" t="str">
+      <c r="C17" s="5" t="str">
         <f ca="1">IF(LEN(C16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,C16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D17" s="6" t="str">
+      <c r="D17" s="5" t="str">
         <f ca="1">IF(LEN(D16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,D16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E17" s="6" t="str">
+      <c r="E17" s="5" t="str">
         <f ca="1">IF(LEN(E16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,E16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F17" s="6" t="str">
+      <c r="F17" s="5" t="str">
         <f ca="1">IF(LEN(F16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,F16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G17" s="6" t="str">
+      <c r="G17" s="5" t="str">
         <f ca="1">IF(LEN(G16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,G16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H17" s="6" t="str">
+      <c r="H17" s="5" t="str">
         <f ca="1">IF(LEN(H16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΜηνΈτους,ΑρΜΜήνα,H16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
@@ -2353,10 +2624,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2372,408 +2643,408 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>9</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <f ca="1">YEAR(TODAY())</f>
         <v>2019</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:8" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="28.2" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="str">
+      <c r="B5" s="6" t="str">
         <f t="shared" ref="B5:H5" ca="1" si="0">IF(WEEKDAY(DATEVALUE(" 1/ "&amp;ΕβδΜήνα&amp;" / "&amp;ΕβδΈτους)-1)=COLUMN(A$2),1,IF(LEN(A5)&gt;0,A5+1,""))</f>
         <v/>
       </c>
-      <c r="C5" s="7" t="str">
+      <c r="C5" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="D5" s="7" t="str">
+      <c r="D5" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="E5" s="7" t="str">
+      <c r="E5" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="F5" s="7" t="str">
+      <c r="F5" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="G5" s="7" t="str">
+      <c r="G5" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="27.6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <f ca="1">IF(LEN(H5)&gt;0,IF(H5=ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",H5+1),"")</f>
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f t="shared" ref="C6:H10" ca="1" si="1">IF(LEN(B6)&gt;0,IF(B6=ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",B6+1),"")</f>
         <v>3</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="27.6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f ca="1">IF(LEN(H6)&gt;0,IF(H6=ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",H6+1),"")</f>
         <v>9</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>13</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>14</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="27.6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <f ca="1">IF(LEN(H7)&gt;0,IF(H7=ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",H7+1),"")</f>
         <v>16</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>17</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>19</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>21</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="27.6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f ca="1">IF(LEN(H8)&gt;0,IF(H8=ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",H8+1),"")</f>
         <v>23</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>25</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>26</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>27</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>28</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="28.2" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <f ca="1">IF(LEN(H9)&gt;0,IF(H9=ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",H9+1),"")</f>
         <v>30</v>
       </c>
-      <c r="C10" s="7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="D10" s="7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="E10" s="7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="F10" s="7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G10" s="7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="H10" s="7" t="str">
+      <c r="C10" s="6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="D10" s="6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F10" s="6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="G10" s="6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H10" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:8" ht="24.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="str">
+      <c r="B12" s="10" t="str">
         <f t="shared" ref="B12:H12" ca="1" si="2">IF(B14="",IF(AND(ISNUMBER(A12),A12&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),A12+1,""),IF(B14&lt;=7,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(A$2))-7))</f>
         <v/>
       </c>
-      <c r="C12" s="11" t="str">
+      <c r="C12" s="10" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="D12" s="11" t="str">
+      <c r="D12" s="10" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="E12" s="11" t="str">
+      <c r="E12" s="10" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="F12" s="11" t="str">
+      <c r="F12" s="10" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="G12" s="11" t="str">
+      <c r="G12" s="10" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="H12" s="11" t="str">
+      <c r="H12" s="10" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="str">
+      <c r="B13" s="11" t="str">
         <f ca="1">IF(LEN(B12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,B12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C13" s="12" t="str">
+      <c r="C13" s="11" t="str">
         <f ca="1">IF(LEN(C12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,C12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D13" s="12" t="str">
+      <c r="D13" s="11" t="str">
         <f ca="1">IF(LEN(D12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,D12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E13" s="12" t="str">
+      <c r="E13" s="11" t="str">
         <f ca="1">IF(LEN(E12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,E12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F13" s="12" t="str">
+      <c r="F13" s="11" t="str">
         <f ca="1">IF(LEN(F12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,F12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G13" s="12" t="str">
+      <c r="G13" s="11" t="str">
         <f ca="1">IF(LEN(G12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,G12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H13" s="12" t="str">
+      <c r="H13" s="11" t="str">
         <f ca="1">IF(LEN(H12)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,H12))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="str">
+      <c r="B14" s="3" t="str">
         <f t="shared" ref="B14:H14" ca="1" si="3">INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(A$2))</f>
         <v/>
       </c>
-      <c r="C14" s="4" t="str">
+      <c r="C14" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="D14" s="4" t="str">
+      <c r="D14" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="E14" s="4" t="str">
+      <c r="E14" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="F14" s="4" t="str">
+      <c r="F14" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="G14" s="4" t="str">
+      <c r="G14" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="str">
+      <c r="B15" s="4" t="str">
         <f ca="1">IF(LEN(B14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,B14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C15" s="5" t="str">
+      <c r="C15" s="4" t="str">
         <f ca="1">IF(LEN(C14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,C14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D15" s="5" t="str">
+      <c r="D15" s="4" t="str">
         <f ca="1">IF(LEN(D14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,D14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E15" s="5" t="str">
+      <c r="E15" s="4" t="str">
         <f ca="1">IF(LEN(E14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,E14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F15" s="5" t="str">
+      <c r="F15" s="4" t="str">
         <f ca="1">IF(LEN(F14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,F14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G15" s="5" t="str">
+      <c r="G15" s="4" t="str">
         <f ca="1">IF(LEN(G14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,G14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H15" s="5" t="str">
+      <c r="H15" s="4" t="str">
         <f ca="1">IF(LEN(H14)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,H14))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <f t="array" aca="1" ref="B16" ca="1">IFERROR(IF(B14="",IF(AND(ISNUMBER(A16),A16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),A16+1,$H$14+COLUMN(A$2)),IF(B14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(A$2))+7)),"")</f>
         <v>2</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <f t="array" aca="1" ref="C16" ca="1">IFERROR(IF(C14="",IF(AND(ISNUMBER(B16),B16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),B16+1,$H$14+COLUMN(B$2)),IF(C14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(B$2))+7)),"")</f>
         <v>3</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <f t="array" aca="1" ref="D16" ca="1">IFERROR(IF(D14="",IF(AND(ISNUMBER(C16),C16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),C16+1,$H$14+COLUMN(C$2)),IF(D14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(C$2))+7)),"")</f>
         <v>4</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <f t="array" aca="1" ref="E16" ca="1">IFERROR(IF(E14="",IF(AND(ISNUMBER(D16),D16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),D16+1,$H$14+COLUMN(D$2)),IF(E14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(D$2))+7)),"")</f>
         <v>5</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <f t="array" aca="1" ref="F16" ca="1">IFERROR(IF(F14="",IF(AND(ISNUMBER(E16),E16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),E16+1,$H$14+COLUMN(E$2)),IF(F14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(E$2))+7)),"")</f>
         <v>6</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <f t="array" aca="1" ref="G16" ca="1">IFERROR(IF(G14="",IF(AND(ISNUMBER(F16),F16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),F16+1,$H$14+COLUMN(F$2)),IF(G14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(F$2))+7)),"")</f>
         <v>7</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <f t="array" aca="1" ref="H16" ca="1">IFERROR(IF(H14="",IF(AND(ISNUMBER(G16),G16&lt;ΤελευταίαΗμέραΜήνα_Εβδομάδα),G16+1,$H$14+COLUMN(G$2)),IF(H14+7&gt;ΤελευταίαΗμέραΜήνα_Εβδομάδα,"",INDEX(ΠροβΕβδΜήνα,ΕβδΕβδομάδα,COLUMN(G$2))+7)),"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="str">
+      <c r="B17" s="11" t="str">
         <f ca="1">IF(LEN(B16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,B16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="C17" s="12" t="str">
+      <c r="C17" s="11" t="str">
         <f ca="1">IF(LEN(C16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,C16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="D17" s="12" t="str">
+      <c r="D17" s="11" t="str">
         <f ca="1">IF(LEN(D16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,D16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="E17" s="12" t="str">
+      <c r="E17" s="11" t="str">
         <f ca="1">IF(LEN(E16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,E16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="F17" s="12" t="str">
+      <c r="F17" s="11" t="str">
         <f ca="1">IF(LEN(F16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,F16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="G17" s="12" t="str">
+      <c r="G17" s="11" t="str">
         <f ca="1">IF(LEN(G16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,G16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>
-      <c r="H17" s="12" t="str">
+      <c r="H17" s="11" t="str">
         <f ca="1">IF(LEN(H16)=0,"",IF(COUNTIF(Εργασίες[ΕΩΣ],DATE(ΕβδΈτους,ΑρΕβδΜήνα,H16))&gt;0,"Παράδοση εργασίας!",""))</f>
         <v/>
       </c>

</xml_diff>